<commit_message>
feat: recalculate NGAM and biomass composition
</commit_message>
<xml_diff>
--- a/data/biomass/biomassCalculations.xlsx
+++ b/data/biomass/biomassCalculations.xlsx
@@ -5,24 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafa\Desktop\finalPaplaGEM\data\biomass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafa\Desktop\papla-GEM-review\data\biomass\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11130" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
-    <sheet name="biomassCuration" sheetId="2" r:id="rId2"/>
+    <sheet name="biomassCuration" sheetId="3" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Calculations!$H$65</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Calculations!$H$64</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
@@ -30,14 +26,11 @@
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">biomassCuration!$G$58</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Calculations!$H$71</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Calculations!$H$70</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -47,11 +40,8 @@
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -69,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="230">
   <si>
     <t>Nucleotide</t>
   </si>
@@ -239,9 +229,6 @@
     <t>TAG</t>
   </si>
   <si>
-    <t>mg/100 mg</t>
-  </si>
-  <si>
     <t>g/gDCW</t>
   </si>
   <si>
@@ -750,6 +737,18 @@
   </si>
   <si>
     <t>s_3737</t>
+  </si>
+  <si>
+    <t>mg/100 mg CDW</t>
+  </si>
+  <si>
+    <t>Total Biomass Fractions</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -825,7 +824,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -892,17 +891,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -932,7 +920,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1037,7 +1025,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1048,31 +1035,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1090,27 +1071,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Protein"/>
-      <sheetName val="Lipid"/>
-      <sheetName val="Carbohydrate"/>
-      <sheetName val="RNA"/>
-      <sheetName val="DNA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1410,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N76"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1419,7 @@
       <c r="B2" s="8">
         <v>331.2</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="41">
         <v>0.24804952027277299</v>
       </c>
       <c r="D2" s="8">
@@ -1468,7 +1428,7 @@
       </c>
       <c r="E2" s="21">
         <f>$G$6*C2</f>
-        <v>8.5212321006723551E-4</v>
+        <v>1.2245921015454507E-3</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7">
@@ -1492,13 +1452,13 @@
       </c>
       <c r="E3" s="21">
         <f>$G$6*C3</f>
-        <v>7.9070442328620929E-4</v>
+        <v>1.1363267423932053E-3</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="41"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -1516,13 +1476,13 @@
       </c>
       <c r="E4" s="21">
         <f>$G$6*C4</f>
-        <v>8.9366072840160217E-4</v>
+        <v>1.284285953642322E-3</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="7">
-        <v>1.1025E-3</v>
-      </c>
-      <c r="J4" s="41"/>
+        <v>1.5844103012372245E-3</v>
+      </c>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -1540,13 +1500,13 @@
       </c>
       <c r="E5" s="21">
         <f>$G$6*C5</f>
-        <v>8.289676880545374E-4</v>
+        <v>1.1913151422643224E-3</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="41"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
@@ -1557,12 +1517,12 @@
       <c r="F6" s="6"/>
       <c r="G6" s="7">
         <f>G4/G2*1000</f>
-        <v>3.4352947311898844E-3</v>
-      </c>
-      <c r="J6" s="41"/>
+        <v>4.9368855871956604E-3</v>
+      </c>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J7" s="41"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J8" s="6"/>
@@ -1611,7 +1571,7 @@
       </c>
       <c r="F10" s="22">
         <f>D10*$G$14</f>
-        <v>9.2758771893410898E-3</v>
+        <v>3.8341842730854657E-3</v>
       </c>
       <c r="G10" s="17">
         <f>SUM(E10:E13)</f>
@@ -1638,7 +1598,7 @@
       </c>
       <c r="F11" s="22">
         <f>D11*$G$14</f>
-        <v>9.2414355667822835E-3</v>
+        <v>3.8199478267786661E-3</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>46</v>
@@ -1664,10 +1624,10 @@
       </c>
       <c r="F12" s="22">
         <f>D12*$G$14</f>
-        <v>9.271250702728712E-3</v>
+        <v>3.8322719146263434E-3</v>
       </c>
       <c r="G12" s="17">
-        <v>1.2578715118241018E-2</v>
+        <v>5.1994124865519104E-3</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1690,7 +1650,7 @@
       </c>
       <c r="F13" s="22">
         <f>D13*$G$14</f>
-        <v>9.2658245764549382E-3</v>
+        <v>3.8300290250755211E-3</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>41</v>
@@ -1713,7 +1673,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="7">
         <f>G12/G10*1000</f>
-        <v>3.7054388035307022E-2</v>
+        <v>1.5316433039565995E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1760,7 +1720,7 @@
       </c>
       <c r="F18" s="22">
         <f t="shared" ref="F18:F37" si="5">D18*$G$22</f>
-        <v>0.14179938761455727</v>
+        <v>0.14099370013794099</v>
       </c>
       <c r="G18" s="17">
         <f>SUM(E18:E37)</f>
@@ -1787,7 +1747,7 @@
       </c>
       <c r="F19" s="22">
         <f t="shared" si="5"/>
-        <v>0.13622091687804755</v>
+        <v>0.13544692561737892</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>48</v>
@@ -1813,10 +1773,10 @@
       </c>
       <c r="F20" s="22">
         <f t="shared" si="5"/>
-        <v>0.11314939725875628</v>
+        <v>0.11250649566452753</v>
       </c>
       <c r="G20" s="17">
-        <v>0.31924513933509435</v>
+        <v>0.31743122592503037</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1839,7 +1799,7 @@
       </c>
       <c r="F21" s="22">
         <f t="shared" si="5"/>
-        <v>0.1322952264999141</v>
+        <v>0.13154354055119316</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>49</v>
@@ -1865,11 +1825,11 @@
       </c>
       <c r="F22" s="22">
         <f t="shared" si="5"/>
-        <v>5.1610965122411298E-2</v>
+        <v>5.1317717676461559E-2</v>
       </c>
       <c r="G22" s="7">
         <f>G20/G18*1000</f>
-        <v>2.3828967557429346</v>
+        <v>2.3693574160710997</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1892,7 +1852,7 @@
       </c>
       <c r="F23" s="22">
         <f t="shared" si="5"/>
-        <v>0.12182582008625181</v>
+        <v>0.12113362007591887</v>
       </c>
       <c r="G23" s="15"/>
     </row>
@@ -1916,7 +1876,7 @@
       </c>
       <c r="F24" s="22">
         <f t="shared" si="5"/>
-        <v>0.13162386873607121</v>
+        <v>0.13087599736336331</v>
       </c>
       <c r="G24" s="15"/>
     </row>
@@ -1940,7 +1900,7 @@
       </c>
       <c r="F25" s="22">
         <f t="shared" si="5"/>
-        <v>0.13880658794441431</v>
+        <v>0.13801790520424168</v>
       </c>
       <c r="G25" s="15"/>
     </row>
@@ -1964,7 +1924,7 @@
       </c>
       <c r="F26" s="22">
         <f t="shared" si="5"/>
-        <v>9.8452324284027212E-2</v>
+        <v>9.7892929733360876E-2</v>
       </c>
       <c r="G26" s="15"/>
     </row>
@@ -1988,7 +1948,7 @@
       </c>
       <c r="F27" s="22">
         <f t="shared" si="5"/>
-        <v>0.12638512120536149</v>
+        <v>0.12566701578122116</v>
       </c>
       <c r="G27" s="15"/>
     </row>
@@ -2012,7 +1972,7 @@
       </c>
       <c r="F28" s="22">
         <f t="shared" si="5"/>
-        <v>0.14001988510798577</v>
+        <v>0.13922430855574139</v>
       </c>
       <c r="G28" s="15"/>
     </row>
@@ -2036,7 +1996,7 @@
       </c>
       <c r="F29" s="22">
         <f t="shared" si="5"/>
-        <v>0.12386685553697095</v>
+        <v>0.12316305860277509</v>
       </c>
       <c r="G29" s="15"/>
     </row>
@@ -2060,7 +2020,7 @@
       </c>
       <c r="F30" s="22">
         <f t="shared" si="5"/>
-        <v>9.6672821777455717E-2</v>
+        <v>9.6123538151161272E-2</v>
       </c>
       <c r="G30" s="15"/>
     </row>
@@ -2084,7 +2044,7 @@
       </c>
       <c r="F31" s="22">
         <f t="shared" si="5"/>
-        <v>0.11405532580755631</v>
+        <v>0.11340727683364731</v>
       </c>
       <c r="G31" s="15"/>
     </row>
@@ -2108,7 +2068,7 @@
       </c>
       <c r="F32" s="22">
         <f t="shared" si="5"/>
-        <v>0.13324159828749982</v>
+        <v>0.13248453516536293</v>
       </c>
       <c r="G32" s="15"/>
     </row>
@@ -2132,7 +2092,7 @@
       </c>
       <c r="F33" s="22">
         <f t="shared" si="5"/>
-        <v>0.13941054031028099</v>
+        <v>0.13861842598365487</v>
       </c>
       <c r="G33" s="15"/>
     </row>
@@ -2156,7 +2116,7 @@
       </c>
       <c r="F34" s="22">
         <f t="shared" si="5"/>
-        <v>0.13488359378219991</v>
+        <v>0.13411720103439256</v>
       </c>
       <c r="G34" s="15"/>
     </row>
@@ -2180,7 +2140,7 @@
       </c>
       <c r="F35" s="22">
         <f t="shared" si="5"/>
-        <v>7.2299029869264397E-2</v>
+        <v>7.1888235267700176E-2</v>
       </c>
       <c r="G35" s="15"/>
     </row>
@@ -2204,7 +2164,7 @@
       </c>
       <c r="F36" s="22">
         <f t="shared" si="5"/>
-        <v>9.9560469026755805E-2</v>
+        <v>9.8994778127730609E-2</v>
       </c>
       <c r="G36" s="15"/>
     </row>
@@ -2228,7 +2188,7 @@
       </c>
       <c r="F37" s="22">
         <f t="shared" si="5"/>
-        <v>0.13671702060715235</v>
+        <v>0.13594021054332547</v>
       </c>
       <c r="G37" s="15"/>
     </row>
@@ -2266,13 +2226,13 @@
     </row>
     <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>1</v>
@@ -2284,102 +2244,105 @@
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B42" s="30">
-        <v>9.4886389353193401</v>
-      </c>
-      <c r="C42" s="43">
-        <v>9.4886389353193393E-2</v>
+        <v>11.3655955879641</v>
+      </c>
+      <c r="C42" s="42">
+        <f>B42/100</f>
+        <v>0.113655955879641</v>
       </c>
       <c r="D42" s="10">
         <v>180.16</v>
       </c>
       <c r="E42" s="23">
         <f>C42/D42*1000</f>
-        <v>0.52667844889649973</v>
-      </c>
-      <c r="G42" s="44"/>
+        <v>0.63086121158770536</v>
+      </c>
+      <c r="G42" s="43"/>
       <c r="N42" s="29"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B43" s="30">
-        <v>1.1873962481112594</v>
-      </c>
-      <c r="C43" s="43">
-        <v>1.1873962481112594E-2</v>
+        <v>0.53855443208978149</v>
+      </c>
+      <c r="C43" s="42">
+        <f t="shared" ref="C43:C44" si="6">B43/100</f>
+        <v>5.3855443208978152E-3</v>
       </c>
       <c r="D43" s="10">
         <v>180.16</v>
       </c>
       <c r="E43" s="23">
         <f>C43/D43*1000</f>
-        <v>6.5907873452001525E-2</v>
-      </c>
-      <c r="G43" s="44"/>
+        <v>2.9893119010312028E-2</v>
+      </c>
+      <c r="G43" s="43"/>
       <c r="N43" s="29"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B44" s="30">
-        <v>7.8076711701176249</v>
-      </c>
-      <c r="C44" s="43">
-        <v>7.8076711701176249E-2</v>
+        <v>6.9006442171887157</v>
+      </c>
+      <c r="C44" s="42">
+        <f t="shared" si="6"/>
+        <v>6.9006442171887158E-2</v>
       </c>
       <c r="D44" s="10">
         <v>342.29599999999999</v>
       </c>
       <c r="E44" s="23">
         <f>C44/D44*1000</f>
-        <v>0.22809706131878915</v>
-      </c>
-      <c r="G44" s="44"/>
+        <v>0.20159873960515801</v>
+      </c>
+      <c r="G44" s="43"/>
       <c r="N44" s="29"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B45" s="50">
-        <v>3.4163051351639724</v>
-      </c>
-      <c r="C45" s="43">
+        <v>5.1865037529013902</v>
+      </c>
+      <c r="C45" s="42">
         <f>(B45/2)/100</f>
-        <v>1.7081525675819862E-2</v>
+        <v>2.5932518764506952E-2</v>
       </c>
       <c r="D45" s="10">
         <v>180.16</v>
       </c>
       <c r="E45" s="23">
         <f>C45/D45*1000</f>
-        <v>9.4813086566495688E-2</v>
-      </c>
-      <c r="G45" s="44"/>
+        <v>0.14394160060228103</v>
+      </c>
+      <c r="G45" s="43"/>
       <c r="N45" s="29"/>
     </row>
     <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B46" s="51"/>
-      <c r="C46" s="43">
+      <c r="C46" s="42">
         <f>(B45/2)/100</f>
-        <v>1.7081525675819862E-2</v>
+        <v>2.5932518764506952E-2</v>
       </c>
       <c r="D46" s="10">
         <v>180.16</v>
       </c>
       <c r="E46" s="23">
         <f>C46/D46*1000</f>
-        <v>9.4813086566495688E-2</v>
-      </c>
-      <c r="G46" s="44"/>
+        <v>0.14394160060228103</v>
+      </c>
+      <c r="G46" s="43"/>
       <c r="N46" s="29"/>
     </row>
     <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2387,42 +2350,42 @@
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="32"/>
       <c r="F48" s="37"/>
       <c r="G48" s="28"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="20"/>
+      <c r="D49" s="39"/>
       <c r="E49" s="38"/>
       <c r="F49" s="38"/>
       <c r="G49" s="38"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="B50" s="47">
+        <v>215</v>
+      </c>
+      <c r="B50" s="45">
         <f>C50*100</f>
-        <v>2.8017329999999996</v>
+        <v>1.17432007</v>
       </c>
       <c r="C50" s="23">
-        <v>2.8017329999999997E-2</v>
-      </c>
-      <c r="D50" s="40"/>
+        <v>1.1743200699999999E-2</v>
+      </c>
+      <c r="D50" s="32"/>
       <c r="E50" s="31"/>
       <c r="F50" s="33"/>
       <c r="G50" s="33"/>
@@ -2431,14 +2394,14 @@
       <c r="A51" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="47">
-        <f t="shared" ref="B51:B60" si="6">C51*100</f>
-        <v>31.358688000000001</v>
+      <c r="B51" s="45">
+        <f t="shared" ref="B51:B60" si="7">C51*100</f>
+        <v>13.143699519999998</v>
       </c>
       <c r="C51" s="23">
-        <v>0.31358688000000001</v>
-      </c>
-      <c r="D51" s="10"/>
+        <v>0.13143699519999999</v>
+      </c>
+      <c r="D51" s="48"/>
       <c r="E51" s="31"/>
       <c r="F51" s="33"/>
       <c r="G51" s="33"/>
@@ -2447,14 +2410,14 @@
       <c r="A52" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="47">
-        <f t="shared" si="6"/>
-        <v>5.1372300000000006</v>
+      <c r="B52" s="45">
+        <f t="shared" si="7"/>
+        <v>2.1532217</v>
       </c>
       <c r="C52" s="23">
-        <v>5.1372300000000003E-2</v>
-      </c>
-      <c r="D52" s="10"/>
+        <v>2.1532216999999999E-2</v>
+      </c>
+      <c r="D52" s="31"/>
       <c r="E52" s="31"/>
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
@@ -2463,14 +2426,14 @@
       <c r="A53" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="47">
-        <f t="shared" si="6"/>
-        <v>0.35040775215364106</v>
+      <c r="B53" s="45">
+        <f t="shared" si="7"/>
+        <v>0.14687011790117274</v>
       </c>
       <c r="C53" s="23">
-        <v>3.5040775215364104E-3</v>
-      </c>
-      <c r="D53" s="10"/>
+        <v>1.4687011790117275E-3</v>
+      </c>
+      <c r="D53" s="31"/>
       <c r="E53" s="31"/>
       <c r="F53" s="33"/>
       <c r="G53" s="33"/>
@@ -2479,14 +2442,14 @@
       <c r="A54" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="47">
-        <f t="shared" si="6"/>
-        <v>0.27068539153972648</v>
+      <c r="B54" s="45">
+        <f t="shared" si="7"/>
+        <v>0.11345523928972141</v>
       </c>
       <c r="C54" s="23">
-        <v>2.7068539153972649E-3</v>
-      </c>
-      <c r="D54" s="10"/>
+        <v>1.1345523928972142E-3</v>
+      </c>
+      <c r="D54" s="31"/>
       <c r="E54" s="31"/>
       <c r="F54" s="33"/>
       <c r="G54" s="33"/>
@@ -2495,14 +2458,14 @@
       <c r="A55" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="47">
-        <f t="shared" si="6"/>
-        <v>0.22433512684996584</v>
+      <c r="B55" s="45">
+        <f t="shared" si="7"/>
+        <v>9.402796121754313E-2</v>
       </c>
       <c r="C55" s="23">
-        <v>2.2433512684996585E-3</v>
-      </c>
-      <c r="D55" s="10"/>
+        <v>9.4027961217543125E-4</v>
+      </c>
+      <c r="D55" s="31"/>
       <c r="E55" s="31"/>
       <c r="F55" s="33"/>
       <c r="G55" s="33"/>
@@ -2511,124 +2474,137 @@
       <c r="A56" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="47">
-        <f t="shared" si="6"/>
-        <v>0.88807052457485469</v>
+      <c r="B56" s="45">
+        <f t="shared" si="7"/>
+        <v>0.37222641864291856</v>
       </c>
       <c r="C56" s="23">
-        <v>8.8807052457485474E-3</v>
-      </c>
-      <c r="D56" s="10"/>
+        <v>3.7222641864291858E-3</v>
+      </c>
+      <c r="D56" s="48"/>
       <c r="E56" s="31"/>
       <c r="F56" s="33"/>
       <c r="G56" s="33"/>
     </row>
     <row r="57" spans="1:12" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="B57" s="47">
-        <f t="shared" si="6"/>
-        <v>4.0788204881811972E-2</v>
+        <v>205</v>
+      </c>
+      <c r="B57" s="45">
+        <f t="shared" si="7"/>
+        <v>1.7095992948644202E-2</v>
       </c>
       <c r="C57" s="23">
-        <v>4.0788204881811972E-4</v>
-      </c>
-      <c r="D57" s="10"/>
+        <v>1.7095992948644204E-4</v>
+      </c>
+      <c r="D57" s="31"/>
       <c r="E57" s="34"/>
       <c r="F57" s="34"/>
       <c r="G57" s="34"/>
     </row>
     <row r="58" spans="1:12" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="B58" s="47">
+        <v>217</v>
+      </c>
+      <c r="B58" s="45">
         <f>C58*100</f>
         <v>0</v>
       </c>
       <c r="C58" s="23">
         <v>0</v>
       </c>
-      <c r="D58" s="10"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="34"/>
       <c r="F58" s="34"/>
       <c r="G58" s="34"/>
     </row>
     <row r="59" spans="1:12" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B59" s="47">
-        <f t="shared" si="6"/>
-        <v>2.1153300000000002</v>
+        <v>218</v>
+      </c>
+      <c r="B59" s="45">
+        <f t="shared" si="7"/>
+        <v>0.88662069999999993</v>
       </c>
       <c r="C59" s="23">
-        <v>2.11533E-2</v>
-      </c>
-      <c r="D59" s="10"/>
+        <v>8.8662069999999992E-3</v>
+      </c>
+      <c r="D59" s="48"/>
       <c r="E59" s="34"/>
       <c r="F59" s="34"/>
       <c r="G59" s="34"/>
     </row>
     <row r="60" spans="1:12" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B60" s="47">
-        <f t="shared" si="6"/>
+        <v>219</v>
+      </c>
+      <c r="B60" s="45">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C60" s="23">
         <v>0</v>
       </c>
-      <c r="D60" s="10"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="34"/>
       <c r="F60" s="34"/>
       <c r="G60" s="34"/>
     </row>
-    <row r="61" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="52"/>
-      <c r="B61" s="53"/>
-      <c r="C61" s="54"/>
-      <c r="D61" s="31"/>
+    <row r="61" spans="1:12" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="34"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
       <c r="E61" s="34"/>
       <c r="F61" s="34"/>
       <c r="G61" s="34"/>
     </row>
-    <row r="62" spans="1:12" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="34"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="34"/>
+    <row r="62" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I62" s="39"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="39"/>
+      <c r="L62" s="32"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>209</v>
+      <c r="A63" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="30">
+        <v>6.4254999999999993E-2</v>
+      </c>
+      <c r="C63" s="42">
+        <v>7.8819906326595773E-2</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="42">
+        <v>0.18094253976454405</v>
       </c>
       <c r="I63" s="39"/>
       <c r="J63" s="39"/>
@@ -2637,91 +2613,100 @@
     </row>
     <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
-        <v>207</v>
+        <v>57</v>
       </c>
       <c r="B64" s="30">
-        <v>0.15335999999999997</v>
-      </c>
-      <c r="C64" s="43">
-        <v>0.18812000000000001</v>
-      </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
+        <v>0.13756000000000002</v>
+      </c>
+      <c r="C64" s="42">
+        <v>1.0131689559660498E-2</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
       <c r="G64" s="10"/>
-      <c r="H64" s="43">
-        <v>0.43165277419425002</v>
-      </c>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="32"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="32"/>
     </row>
     <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B65" s="30">
-        <v>0.32832</v>
-      </c>
-      <c r="C65" s="43">
-        <v>2.418E-2</v>
-      </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-      <c r="H65" s="33"/>
+        <v>4.596495</v>
+      </c>
+      <c r="C65" s="42">
+        <v>4.0755155502095561E-2</v>
+      </c>
+      <c r="D65" s="30">
+        <f>(100/SUM($B$65,$B$67:$B$69))*B65</f>
+        <v>25.92914028997345</v>
+      </c>
+      <c r="E65" s="30">
+        <f>(100/SUM($B$65,$B$67:$B$69))*C65</f>
+        <v>0.22990259851332789</v>
+      </c>
+      <c r="F65" s="23">
+        <f>(D65/100)*$H$63</f>
+        <v>4.6916844979789624E-2</v>
+      </c>
+      <c r="G65" s="23">
+        <f>(E65/100)*$H$63</f>
+        <v>4.1599160073469836E-4</v>
+      </c>
+      <c r="H65" s="47"/>
       <c r="I65" s="33"/>
       <c r="J65" s="32"/>
       <c r="K65" s="32"/>
     </row>
     <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="26" t="s">
-        <v>59</v>
+      <c r="A66" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="B66" s="30">
-        <v>10.97064</v>
-      </c>
-      <c r="C66" s="43">
-        <v>9.7269999999999995E-2</v>
-      </c>
-      <c r="D66" s="30">
-        <f>(100/SUM($B$66,$B$68:$B$70))*B66</f>
-        <v>25.929140289973454</v>
-      </c>
-      <c r="E66" s="30">
-        <f>(100/SUM($B$66,$B$68:$B$70))*C66</f>
-        <v>0.22989793448747911</v>
-      </c>
-      <c r="F66" s="23">
-        <f>(D66/100)*$H$64</f>
-        <v>0.11192385338638941</v>
-      </c>
-      <c r="G66" s="23">
-        <f>(E66/100)*$H$64</f>
-        <v>9.9236081203048308E-4</v>
-      </c>
-      <c r="H66" s="49"/>
+        <v>0.1135775</v>
+      </c>
+      <c r="C66" s="42">
+        <v>1.2745193538480833E-2</v>
+      </c>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="47"/>
       <c r="I66" s="33"/>
       <c r="J66" s="32"/>
       <c r="K66" s="32"/>
     </row>
     <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="10" t="s">
-        <v>208</v>
+      <c r="A67" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="B67" s="30">
-        <v>0.27107999999999993</v>
-      </c>
-      <c r="C67" s="43">
-        <v>3.0419999999999999E-2</v>
-      </c>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="49"/>
+        <v>1.0122424999999999</v>
+      </c>
+      <c r="C67" s="42">
+        <v>3.4639163168298431E-2</v>
+      </c>
+      <c r="D67" s="30">
+        <f t="shared" ref="D67:E69" si="8">(100/SUM($B$65,$B$67:$B$69))*B67</f>
+        <v>5.7101286501939956</v>
+      </c>
+      <c r="E67" s="30">
+        <f t="shared" si="8"/>
+        <v>0.1954018706249199</v>
+      </c>
+      <c r="F67" s="23">
+        <f t="shared" ref="F67:G68" si="9">(D67/100)*$H$63</f>
+        <v>1.0332051803483892E-2</v>
+      </c>
+      <c r="G67" s="23">
+        <f t="shared" si="9"/>
+        <v>3.5356510745615863E-4</v>
+      </c>
+      <c r="H67" s="47"/>
       <c r="I67" s="33"/>
       <c r="J67" s="32"/>
       <c r="K67" s="32"/>
@@ -2731,28 +2716,28 @@
         <v>60</v>
       </c>
       <c r="B68" s="30">
-        <v>2.4159599999999997</v>
-      </c>
-      <c r="C68" s="43">
-        <v>8.2669999999999993E-2</v>
+        <v>5.3969675000000006</v>
+      </c>
+      <c r="C68" s="42">
+        <v>0.23308215996010256</v>
       </c>
       <c r="D68" s="30">
-        <f t="shared" ref="D68:E70" si="7">(100/SUM($B$66,$B$68:$B$70))*B68</f>
-        <v>5.7101286501939965</v>
+        <f t="shared" si="8"/>
+        <v>30.444659995915867</v>
       </c>
       <c r="E68" s="30">
-        <f t="shared" si="7"/>
-        <v>0.19539079103608409</v>
+        <f t="shared" si="8"/>
+        <v>1.3148322851858931</v>
       </c>
       <c r="F68" s="23">
-        <f t="shared" ref="F68:G69" si="8">(D68/100)*$H$64</f>
-        <v>2.4647928728623068E-2</v>
+        <f t="shared" si="9"/>
+        <v>5.5087341019290303E-2</v>
       </c>
       <c r="G68" s="23">
-        <f t="shared" si="8"/>
-        <v>8.4340977002734694E-4</v>
-      </c>
-      <c r="H68" s="49"/>
+        <f t="shared" si="9"/>
+        <v>2.3790909304595479E-3</v>
+      </c>
+      <c r="H68" s="47"/>
       <c r="I68" s="33"/>
       <c r="J68" s="32"/>
       <c r="K68" s="32"/>
@@ -2762,98 +2747,120 @@
         <v>61</v>
       </c>
       <c r="B69" s="30">
-        <v>12.881159999999999</v>
-      </c>
-      <c r="C69" s="43">
-        <v>0.55630999999999997</v>
+        <v>6.7214350000000005</v>
+      </c>
+      <c r="C69" s="42">
+        <v>0.132262171336579</v>
       </c>
       <c r="D69" s="30">
-        <f t="shared" si="7"/>
-        <v>30.44465999591587</v>
+        <f t="shared" si="8"/>
+        <v>37.916071063916682</v>
       </c>
       <c r="E69" s="30">
-        <f t="shared" si="7"/>
-        <v>1.3148403406469571</v>
+        <f t="shared" si="8"/>
+        <v>0.74609988603113064</v>
       </c>
       <c r="F69" s="23">
-        <f t="shared" si="8"/>
-        <v>0.13141521946637788</v>
+        <f>(D69/100)*$H$63</f>
+        <v>6.8606301961980226E-2</v>
       </c>
       <c r="G69" s="23">
-        <f t="shared" si="8"/>
-        <v>5.6755448066277171E-3</v>
-      </c>
-      <c r="H69" s="49"/>
+        <f>(E69/100)*$H$63</f>
+        <v>1.3500120829650964E-3</v>
+      </c>
+      <c r="H69" s="47"/>
       <c r="I69" s="33"/>
-      <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
-    </row>
-    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="26" t="s">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
+      <c r="B70" s="44">
+        <f>SUM(B63:B69)</f>
+        <v>18.0425325</v>
+      </c>
+      <c r="C70" s="31"/>
+      <c r="D70" s="44">
+        <f>SUM(D65:D69)</f>
+        <v>100</v>
+      </c>
+      <c r="E70" s="44"/>
+      <c r="F70" s="31">
+        <f>SUM(F65:F69)</f>
+        <v>0.18094253976454405</v>
+      </c>
+      <c r="G70" s="46"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="32"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="32"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="32"/>
+      <c r="G71" s="32"/>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="30">
-        <v>16.04232</v>
-      </c>
-      <c r="C70" s="43">
-        <v>0.31568000000000002</v>
-      </c>
-      <c r="D70" s="30">
-        <f t="shared" si="7"/>
-        <v>37.916071063916689</v>
-      </c>
-      <c r="E70" s="30">
-        <f t="shared" si="7"/>
-        <v>0.74611061950249224</v>
-      </c>
-      <c r="F70" s="23">
-        <f>(D70/100)*$H$64</f>
-        <v>0.16366577261285969</v>
-      </c>
-      <c r="G70" s="23">
-        <f>(E70/100)*$H$64</f>
-        <v>3.2206071876404131E-3</v>
-      </c>
-      <c r="H70" s="49"/>
-      <c r="I70" s="33"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="46">
-        <f>SUM(D66:D70)</f>
-        <v>100.00000000000001</v>
-      </c>
-      <c r="E71" s="46"/>
-      <c r="F71" s="31">
-        <f>SUM(F66:F70)</f>
-        <v>0.43165277419425002</v>
-      </c>
-      <c r="G71" s="48"/>
-      <c r="H71" s="32"/>
-      <c r="I71" s="32"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="32"/>
-      <c r="B72" s="32"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="33"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="32"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G73"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74" s="49">
+        <v>0.15840000000000001</v>
+      </c>
       <c r="G74"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" s="49">
+        <v>0.51990000000000003</v>
+      </c>
       <c r="G75"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G76"/>
+    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B76" s="18">
+        <v>31.74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B77" s="18">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B78" s="18">
+        <v>18.09</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="B79" s="49">
+        <v>25.5017</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A18:F37">
@@ -2871,28 +2878,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>66</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,14 +2907,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="45">
-        <f>-Calculations!E2</f>
-        <v>-8.5212321006723551E-4</v>
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>-1.224592E-3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2915,14 +2921,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="45">
-        <f>-Calculations!E3</f>
-        <v>-7.9070442328620929E-4</v>
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>-1.1363269999999999E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2930,14 +2935,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="45">
-        <f>-Calculations!E4</f>
-        <v>-8.9366072840160217E-4</v>
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>-1.2842859999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2945,1067 +2949,997 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="45">
-        <f>-Calculations!E5</f>
-        <v>-8.289676880545374E-4</v>
+      <c r="D5">
+        <v>-1.1913150000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
         <v>91</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D7">
+        <v>-3.834184E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8">
+        <v>-3.8199480000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9">
+        <v>-3.8322719999999998E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10">
+        <v>-3.830029E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
         <v>186</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="45">
-        <f>-Calculations!F10</f>
-        <v>-9.2758771893410898E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="45">
-        <f>-Calculations!F11</f>
-        <v>-9.2414355667822835E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="45">
-        <f>-Calculations!F12</f>
-        <v>-9.271250702728712E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="28" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12">
+        <v>0.1409937</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13">
+        <v>0.135446926</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14">
+        <v>0.112506496</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15">
+        <v>0.13154354100000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16">
+        <v>5.1317717999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17">
+        <v>0.12113362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18">
+        <v>0.13087599699999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19">
+        <v>0.138017905</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20">
+        <v>9.7892930000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21">
+        <v>0.12566701599999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22">
+        <v>0.13922430899999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23">
+        <v>0.12316305900000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24">
+        <v>9.6123537999999994E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25">
+        <v>0.113407277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26">
+        <v>0.13248453499999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27">
+        <v>0.13861842599999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28">
+        <v>0.13411720099999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29">
+        <v>7.1888234999999995E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30">
+        <v>9.8994778000000005E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31">
+        <v>0.13594021100000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" t="s">
         <v>99</v>
       </c>
-      <c r="C10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="45">
-        <f>-Calculations!F13</f>
-        <v>-9.2658245764549382E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="C11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="45">
-        <f>Calculations!F18</f>
-        <v>0.14179938761455727</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="45">
-        <f>Calculations!F19</f>
-        <v>0.13622091687804755</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="45">
-        <f>Calculations!F20</f>
-        <v>0.11314939725875628</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="45">
-        <f>Calculations!F21</f>
-        <v>0.1322952264999141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="45">
-        <f>Calculations!F22</f>
-        <v>5.1610965122411298E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="45">
-        <f>Calculations!F23</f>
-        <v>0.12182582008625181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="45">
-        <f>Calculations!F24</f>
-        <v>0.13162386873607121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="45">
-        <f>Calculations!F25</f>
-        <v>0.13880658794441431</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="45">
-        <f>Calculations!F26</f>
-        <v>9.8452324284027212E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="45">
-        <f>Calculations!F27</f>
-        <v>0.12638512120536149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="45">
-        <f>Calculations!F28</f>
-        <v>0.14001988510798577</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="45">
-        <f>Calculations!F29</f>
-        <v>0.12386685553697095</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="45">
-        <f>Calculations!F30</f>
-        <v>9.6672821777455717E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="45">
-        <f>Calculations!F31</f>
-        <v>0.11405532580755631</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="45">
-        <f>Calculations!F32</f>
-        <v>0.13324159828749982</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="C27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="45">
-        <f>Calculations!F33</f>
-        <v>0.13941054031028099</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="C28" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="45">
-        <f>Calculations!F34</f>
-        <v>0.13488359378219991</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="C29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="45">
-        <f>Calculations!F35</f>
-        <v>7.2299029869264397E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="45">
-        <f>Calculations!F36</f>
-        <v>9.9560469026755805E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="45">
-        <f>Calculations!F37</f>
-        <v>0.13671702060715235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32">
+        <v>-0.1409937</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B33" t="s">
         <v>100</v>
       </c>
-      <c r="C32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="45">
-        <f>-Calculations!F18</f>
-        <v>-0.14179938761455727</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33">
+        <v>-0.135446926</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B34" t="s">
         <v>101</v>
       </c>
-      <c r="C33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="45">
-        <f>-Calculations!F19</f>
-        <v>-0.13622091687804755</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34">
+        <v>-0.112506496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>162</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B35" t="s">
         <v>102</v>
       </c>
-      <c r="C34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="45">
-        <f>-Calculations!F20</f>
-        <v>-0.11314939725875628</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35">
+        <v>-0.13154354100000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B36" t="s">
         <v>103</v>
       </c>
-      <c r="C35" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="45">
-        <f>-Calculations!F21</f>
-        <v>-0.1322952264999141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36">
+        <v>-5.1317717999999998E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B37" t="s">
         <v>104</v>
       </c>
-      <c r="C36" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="45">
-        <f>-Calculations!F22</f>
-        <v>-5.1610965122411298E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37">
+        <v>-0.12113362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B38" t="s">
         <v>105</v>
       </c>
-      <c r="C37" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="45">
-        <f>-Calculations!F23</f>
-        <v>-0.12182582008625181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38">
+        <v>-0.13087599699999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B39" t="s">
         <v>106</v>
       </c>
-      <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="45">
-        <f>-Calculations!F24</f>
-        <v>-0.13162386873607121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39">
+        <v>-0.138017905</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B40" t="s">
         <v>107</v>
       </c>
-      <c r="C39" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" s="45">
-        <f>-Calculations!F25</f>
-        <v>-0.13880658794441431</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40">
+        <v>-9.7892930000000003E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B41" t="s">
         <v>108</v>
       </c>
-      <c r="C40" t="s">
-        <v>93</v>
-      </c>
-      <c r="D40" s="45">
-        <f>-Calculations!F26</f>
-        <v>-9.8452324284027212E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41">
+        <v>-0.12566701599999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>169</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B42" t="s">
         <v>109</v>
       </c>
-      <c r="C41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="45">
-        <f>-Calculations!F27</f>
-        <v>-0.12638512120536149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="C42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42">
+        <v>-0.13922430899999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B43" t="s">
         <v>110</v>
       </c>
-      <c r="C42" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="45">
-        <f>-Calculations!F28</f>
-        <v>-0.14001988510798577</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43">
+        <v>-0.12316305900000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>171</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B44" t="s">
         <v>111</v>
       </c>
-      <c r="C43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="45">
-        <f>-Calculations!F29</f>
-        <v>-0.12386685553697095</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44">
+        <v>-9.6123537999999994E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>172</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B45" t="s">
         <v>112</v>
       </c>
-      <c r="C44" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="45">
-        <f>-Calculations!F30</f>
-        <v>-9.6672821777455717E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45">
+        <v>-0.113407277</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B46" t="s">
         <v>113</v>
       </c>
-      <c r="C45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="45">
-        <f>-Calculations!F31</f>
-        <v>-0.11405532580755631</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46">
+        <v>-0.13248453499999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>174</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B47" t="s">
         <v>114</v>
       </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="45">
-        <f>-Calculations!F32</f>
-        <v>-0.13324159828749982</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
+      <c r="C47" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47">
+        <v>-0.13861842599999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>175</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B48" t="s">
         <v>115</v>
       </c>
-      <c r="C47" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" s="45">
-        <f>-Calculations!F33</f>
-        <v>-0.13941054031028099</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48">
+        <v>-0.13411720099999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="28" t="s">
+      <c r="B49" t="s">
         <v>116</v>
       </c>
-      <c r="C48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48" s="45">
-        <f>-Calculations!F34</f>
-        <v>-0.13488359378219991</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49">
+        <v>-7.1888234999999995E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>177</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B50" t="s">
         <v>117</v>
       </c>
-      <c r="C49" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49" s="45">
-        <f>-Calculations!F35</f>
-        <v>-7.2299029869264397E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50">
+        <v>-9.8994778000000005E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B51" t="s">
         <v>118</v>
       </c>
-      <c r="C50" t="s">
-        <v>93</v>
-      </c>
-      <c r="D50" s="45">
-        <f>-Calculations!F36</f>
-        <v>-9.9560469026755805E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="C51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51">
+        <v>-0.13594021100000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>179</v>
       </c>
-      <c r="B51" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51" s="45">
-        <f>-Calculations!F37</f>
-        <v>-0.13671702060715235</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
+      <c r="B52" t="s">
         <v>180</v>
       </c>
-      <c r="B52" s="28" t="s">
-        <v>181</v>
-      </c>
       <c r="C52" t="s">
-        <v>93</v>
-      </c>
-      <c r="D52" s="45">
+        <v>92</v>
+      </c>
+      <c r="D52">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
         <v>68</v>
       </c>
-      <c r="B53" t="s">
-        <v>69</v>
-      </c>
       <c r="C53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D53" s="45">
-        <f>-Calculations!C56</f>
-        <v>-8.8807052457485474E-3</v>
+        <v>94</v>
+      </c>
+      <c r="D53">
+        <v>-3.7222639999999999E-3</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
         <v>70</v>
       </c>
-      <c r="B54" t="s">
-        <v>71</v>
-      </c>
       <c r="C54" t="s">
-        <v>95</v>
-      </c>
-      <c r="D54" s="45">
-        <f>-Calculations!C54</f>
-        <v>-2.7068539153972649E-3</v>
+        <v>94</v>
+      </c>
+      <c r="D54">
+        <v>-1.134552E-3</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" t="s">
         <v>72</v>
       </c>
-      <c r="B55" t="s">
-        <v>73</v>
-      </c>
       <c r="C55" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="45">
-        <f>-Calculations!C55</f>
-        <v>-2.2433512684996585E-3</v>
+        <v>94</v>
+      </c>
+      <c r="D55">
+        <v>-9.4028000000000004E-4</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" t="s">
         <v>74</v>
       </c>
-      <c r="B56" t="s">
-        <v>75</v>
-      </c>
       <c r="C56" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="45">
-        <f>-Calculations!C53</f>
-        <v>-3.5040775215364104E-3</v>
+        <v>94</v>
+      </c>
+      <c r="D56">
+        <v>-1.468701E-3</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" t="s">
         <v>76</v>
       </c>
-      <c r="B57" t="s">
-        <v>77</v>
-      </c>
       <c r="C57" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" s="45">
-        <f>-Calculations!C51</f>
-        <v>-0.31358688000000001</v>
+        <v>94</v>
+      </c>
+      <c r="D57">
+        <v>-0.131436995</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" t="s">
         <v>78</v>
       </c>
-      <c r="B58" t="s">
-        <v>79</v>
-      </c>
       <c r="C58" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58" s="45">
-        <f>-Calculations!C50</f>
-        <v>-2.8017329999999997E-2</v>
+        <v>94</v>
+      </c>
+      <c r="D58">
+        <v>-1.1743201E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" t="s">
         <v>80</v>
       </c>
-      <c r="B59" t="s">
-        <v>81</v>
-      </c>
       <c r="C59" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="45">
-        <f>-Calculations!C52</f>
-        <v>-5.1372300000000003E-2</v>
+        <v>94</v>
+      </c>
+      <c r="D59">
+        <v>-2.1532216999999999E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>210</v>
+      </c>
+      <c r="B60" t="s">
         <v>211</v>
       </c>
-      <c r="B60" t="s">
-        <v>212</v>
-      </c>
       <c r="C60" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" s="45">
-        <f>-Calculations!C57</f>
-        <v>-4.0788204881811972E-4</v>
+        <v>94</v>
+      </c>
+      <c r="D60">
+        <v>-1.7096E-4</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" s="45">
-        <f>-Calculations!C58</f>
+        <v>94</v>
+      </c>
+      <c r="D61">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B62" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C62" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62" s="45">
-        <f>-Calculations!C59</f>
-        <v>-2.11533E-2</v>
+        <v>94</v>
+      </c>
+      <c r="D62">
+        <v>-8.8662069999999992E-3</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C63" t="s">
-        <v>95</v>
-      </c>
-      <c r="D63" s="45">
-        <f>-Calculations!C60</f>
+        <v>94</v>
+      </c>
+      <c r="D63">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
-      </c>
-      <c r="D64" s="45">
+        <v>94</v>
+      </c>
+      <c r="D64">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" t="s">
         <v>82</v>
       </c>
-      <c r="B65" s="28" t="s">
-        <v>83</v>
-      </c>
       <c r="C65" t="s">
-        <v>94</v>
-      </c>
-      <c r="D65" s="45">
-        <f>-Calculations!F66</f>
-        <v>-0.11192385338638941</v>
+        <v>93</v>
+      </c>
+      <c r="D65">
+        <v>-4.6916844999999999E-2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>212</v>
+      </c>
+      <c r="B66" t="s">
         <v>213</v>
       </c>
-      <c r="B66" s="28" t="s">
-        <v>214</v>
-      </c>
       <c r="C66" t="s">
-        <v>94</v>
-      </c>
-      <c r="D66" s="45">
-        <f>-Calculations!F68</f>
-        <v>-2.4647928728623068E-2</v>
+        <v>93</v>
+      </c>
+      <c r="D66">
+        <v>-1.0332052E-2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
+      <c r="A67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67">
+        <v>-5.5087340999999998E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>85</v>
       </c>
-      <c r="B67" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C67" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="45">
-        <f>-Calculations!F69</f>
-        <v>-0.13141521946637788</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B68" s="28" t="s">
-        <v>210</v>
+      <c r="B68" t="s">
+        <v>209</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
-      </c>
-      <c r="D68" s="45">
-        <f>-Calculations!F70</f>
-        <v>-0.16366577261285969</v>
+        <v>93</v>
+      </c>
+      <c r="D68">
+        <v>-6.8606301999999994E-2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B69" s="28" t="s">
-        <v>185</v>
+      <c r="A69" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" t="s">
+        <v>184</v>
       </c>
       <c r="C69" t="s">
-        <v>94</v>
-      </c>
-      <c r="D69" s="45">
+        <v>93</v>
+      </c>
+      <c r="D69">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="str">
-        <f>Calculations!A42</f>
-        <v>glycogen</v>
-      </c>
-      <c r="B70" s="28" t="s">
+      <c r="A70" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" t="s">
+        <v>201</v>
+      </c>
+      <c r="C70" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70">
+        <v>-0.630861212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>193</v>
+      </c>
+      <c r="B71" t="s">
         <v>202</v>
       </c>
-      <c r="C70" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" s="45">
-        <f>-Calculations!E42</f>
-        <v>-0.52667844889649973</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="str">
-        <f>Calculations!A43</f>
-        <v>mannan</v>
-      </c>
-      <c r="B71" s="28" t="s">
+      <c r="C71" t="s">
+        <v>191</v>
+      </c>
+      <c r="D71">
+        <v>-2.9893118999999999E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>198</v>
+      </c>
+      <c r="B72" t="s">
         <v>203</v>
       </c>
-      <c r="C71" t="s">
-        <v>192</v>
-      </c>
-      <c r="D71" s="45">
-        <f>-Calculations!E43</f>
-        <v>-6.5907873452001525E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="str">
-        <f>Calculations!A44</f>
-        <v>trehalose</v>
-      </c>
-      <c r="B72" s="28" t="s">
-        <v>204</v>
-      </c>
       <c r="C72" t="s">
-        <v>192</v>
-      </c>
-      <c r="D72" s="45">
-        <f>-Calculations!E44</f>
-        <v>-0.22809706131878915</v>
+        <v>191</v>
+      </c>
+      <c r="D72">
+        <v>-0.20159874</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="str">
-        <f>Calculations!A45</f>
-        <v>(1-&gt;3)-beta-D-glucan</v>
+      <c r="A73" t="s">
+        <v>196</v>
       </c>
       <c r="B73" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" t="s">
+        <v>191</v>
+      </c>
+      <c r="D73">
+        <v>-0.143941601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74" t="s">
         <v>200</v>
       </c>
-      <c r="C73" t="s">
-        <v>192</v>
-      </c>
-      <c r="D73" s="45">
-        <f>-Calculations!E45</f>
-        <v>-9.4813086566495688E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="str">
-        <f>Calculations!A46</f>
-        <v>(1-&gt;6)-beta-D-glucan</v>
-      </c>
-      <c r="B74" t="s">
-        <v>201</v>
-      </c>
       <c r="C74" t="s">
-        <v>192</v>
-      </c>
-      <c r="D74" s="45">
-        <f>-Calculations!E46</f>
-        <v>-9.4813086566495688E-2</v>
+        <v>191</v>
+      </c>
+      <c r="D74">
+        <v>-0.143941601</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>192</v>
-      </c>
-      <c r="B75" s="28" t="s">
-        <v>205</v>
+        <v>191</v>
+      </c>
+      <c r="B75" t="s">
+        <v>204</v>
       </c>
       <c r="C75" t="s">
-        <v>192</v>
-      </c>
-      <c r="D75" s="45">
+        <v>191</v>
+      </c>
+      <c r="D75">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>